<commit_message>
4 & 5 Modification 5
</commit_message>
<xml_diff>
--- a/5. Clarify the definition of the system/5.3. Уточнение прецедентов.xlsx
+++ b/5. Clarify the definition of the system/5.3. Уточнение прецедентов.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="72">
   <si>
     <t>Прецендент</t>
   </si>
@@ -37,12 +37,6 @@
     <t>Получение VIP-статуса</t>
   </si>
   <si>
-    <t>Формирование персональных скидок</t>
-  </si>
-  <si>
-    <t>Формирование зарплат</t>
-  </si>
-  <si>
     <t>Клиент</t>
   </si>
   <si>
@@ -58,21 +52,6 @@
     <t>Администратор</t>
   </si>
   <si>
-    <t>Бухгалтерия</t>
-  </si>
-  <si>
-    <t>Бухгалтер запрашивает информацию по определенному клиенту и его заказах и получает персональную скидку</t>
-  </si>
-  <si>
-    <t>Бухгалтер получает персональную скидку по клиенту</t>
-  </si>
-  <si>
-    <t>Система обрабатывает данные по заказам выбранного клиента</t>
-  </si>
-  <si>
-    <t>Бухгалтер получает всю необходимую информацию для формирования зарплат</t>
-  </si>
-  <si>
     <t>Администрирование системы</t>
   </si>
   <si>
@@ -212,12 +191,6 @@
   </si>
   <si>
     <t>Возможность контролировать всю информацию о парковках компании</t>
-  </si>
-  <si>
-    <t>Бухгалтер обращается к базе сотрудников и их окладов и формирует зарплаты</t>
-  </si>
-  <si>
-    <t>Обращение к базе сотрудников и получение информации об их зарплатах</t>
   </si>
   <si>
     <t>Возможность отмены брони</t>
@@ -651,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A16" activeCellId="1" sqref="A17:XFD17 A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -685,87 +658,87 @@
     </row>
     <row r="2" spans="1:5" ht="93.75">
       <c r="A2" s="6" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="112.5">
       <c r="A3" s="6" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="75">
       <c r="A4" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>80</v>
-      </c>
       <c r="E4" s="7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="112.5">
       <c r="A5" s="4" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="56.25">
       <c r="A6" s="4" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="75">
@@ -773,220 +746,186 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="93.75">
       <c r="A8" s="5" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="93.75">
       <c r="A9" s="4" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="56.25">
       <c r="A10" s="5" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="56.25">
       <c r="A11" s="5" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="93.75">
       <c r="A12" s="5" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="93.75">
       <c r="A13" s="5" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="75">
       <c r="A14" s="5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="75">
       <c r="A15" s="5" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="75">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="56.25">
       <c r="A16" s="5" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="93.75">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="75">
       <c r="A17" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>66</v>
-      </c>
       <c r="C17" s="3" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="56.25">
-      <c r="A18" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="75">
-      <c r="A19" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>